<commit_message>
Updates to List of Figures/Tables chapter 3
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41460755-A093-4BBF-8CE8-F877EEC98C62}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4F956B5-CA50-40FF-B995-932307FE51F1}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Supplementary Table S3.1</t>
   </si>
   <si>
-    <t>Table 3.3</t>
-  </si>
-  <si>
     <t>List of eukaryotic species used for the phylogenetic analysis of phototransduction gene families.</t>
   </si>
   <si>
@@ -84,13 +81,28 @@
   </si>
   <si>
     <t>Added to manuscript.</t>
+  </si>
+  <si>
+    <t>Prepared. To be added in github.</t>
+  </si>
+  <si>
+    <t>Online Supplementary Material</t>
+  </si>
+  <si>
+    <t>All Figures, Tables, Files (Main and Supplementary) of Chapter 3 in order of mention in manuscript.</t>
+  </si>
+  <si>
+    <t>Supplementary Table S3.2</t>
+  </si>
+  <si>
+    <t>Number of duplication and loss events for each gene family and comparison Cteno-first vs Sponge-first scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +113,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -127,9 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,6 +165,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,87 +468,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D7" sqref="D7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="110.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated List of Figs/Tables
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4F956B5-CA50-40FF-B995-932307FE51F1}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC7D5DFB-840B-4E7F-AF66-4451E601B424}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Number of duplication and loss events for each gene family and comparison Cteno-first vs Sponge-first scenarios</t>
+  </si>
+  <si>
+    <t>Figure 3.2</t>
+  </si>
+  <si>
+    <t>Evolutionary history of phototransduction components gene families and distribution across Eukarya</t>
   </si>
 </sst>
 </file>
@@ -471,7 +477,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,8 +578,17 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Fig/Table list
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC7D5DFB-840B-4E7F-AF66-4451E601B424}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D27FE5B4-F15C-481A-91AE-F0FA7059AC82}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -102,13 +102,63 @@
   </si>
   <si>
     <t>Evolutionary history of phototransduction components gene families and distribution across Eukarya</t>
+  </si>
+  <si>
+    <t>Figure 3.3</t>
+  </si>
+  <si>
+    <t>Supplementary Figure X</t>
+  </si>
+  <si>
+    <t>NEEDS TO BE PROPERLY PREPAPARED &amp; DECIDED WHERE TO PUT ETC.</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Although mentioned as one Figure, there are actually two reconciliations - sponge first and cteno first</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Supplementary Figure with Full reconciliation for </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">GRK </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Supplementary Figure with Full reconciliation for </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PLC</t>
+    </r>
+  </si>
+  <si>
+    <t>Major events of duplication, speciation, and losses for three phototransduction gene families of interest.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +181,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,16 +228,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -474,121 +577,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="110.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="110.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.54296875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="38" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to figs/tables list
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBD4420B-4BAE-4CFB-AE6E-852AC74DB350}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD27E2F5-ED92-42FB-8F8D-EA47159619F4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>Figure 3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross-species comparison of orthogroups of regulatory genes expressed in PRC-like metacells. </t>
+  </si>
+  <si>
+    <t>Figure 3.8</t>
+  </si>
+  <si>
+    <t>Extended Figure 3.8A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most common orthogroups of regulatory genes shared across PRC-like metacells throughout animals. </t>
   </si>
 </sst>
 </file>
@@ -667,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,8 +954,38 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="9" t="s">
         <v>43</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates list of figs/tables
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E53567B6-B14B-42F0-A947-1C0880EE94A7}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B740368-54BA-4C66-B99E-A3FDF5396F2C}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -221,13 +221,10 @@
     <t>Same as above but for all orthogroups present in at least 2 species.</t>
   </si>
   <si>
-    <t>Excel file.. Probably should remove all the part with the pfams...</t>
-  </si>
-  <si>
     <t>Supplementary Table S3.3</t>
   </si>
   <si>
-    <t>List of all orthogroups in at least 2 metacells and metadata.</t>
+    <t>List of all Eggnog orthogroups and ATFDB annotation.</t>
   </si>
 </sst>
 </file>
@@ -697,7 +694,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1013,22 +1010,20 @@
       </c>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>48</v>
-      </c>
+      <c r="D22" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to figs and tables list
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B740368-54BA-4C66-B99E-A3FDF5396F2C}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F17AA20E-B136-4C9C-8001-507455E897AB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
+    <workbookView minimized="1" xWindow="32100" yWindow="3300" windowWidth="18000" windowHeight="12615" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>List of all Eggnog orthogroups and ATFDB annotation.</t>
+  </si>
+  <si>
+    <t>Species tree with ctenophore first.</t>
+  </si>
+  <si>
+    <t>To be prepared</t>
+  </si>
+  <si>
+    <t>Species tree with sponge first.</t>
   </si>
 </sst>
 </file>
@@ -324,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -367,6 +376,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,6 +1040,36 @@
       </c>
       <c r="E22" s="16"/>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates Methods outline and Notes to the figs/tables list
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22D7553C-0FAE-476F-8D17-CC8CDE1ED03B}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C946B8F-AB7E-4229-AF99-93554D92EFE4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="1" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mentioned_in_text" sheetId="1" r:id="rId1"/>
+    <sheet name="Extra_on_github" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -246,6 +247,18 @@
   </si>
   <si>
     <t>List of models for gene trees</t>
+  </si>
+  <si>
+    <t>Some extra files that do not need to be mentioned in the text but that should anyway be provided in the github:</t>
+  </si>
+  <si>
+    <t>scripts...</t>
+  </si>
+  <si>
+    <t>list of marker genes used for each species in the metacell pipeline.... The gene codes would be present in the metacell script for each species, but perhaps provide also a fasta file?.... Also the description of which categorise... See google sheets files...</t>
+  </si>
+  <si>
+    <t>for the metacell pipelines: in theory I could provide also all the files necessary for people to run the scripts..... Separate directory per species...</t>
   </si>
 </sst>
 </file>
@@ -720,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1116,4 +1129,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BA4A1-55DF-473D-9C92-55227EF915D8}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to Figs/Tables list Chapter 3
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING/3_Evolution_of_phototransduction_and_PRCs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C946B8F-AB7E-4229-AF99-93554D92EFE4}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51ED9736-CD0D-4251-B091-2F264B2A0891}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="1" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentioned_in_text" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>for the metacell pipelines: in theory I could provide also all the files necessary for people to run the scripts..... Separate directory per species...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplementary Figures on GitHub </t>
+  </si>
+  <si>
+    <t>Metacell Pipeline output figures.</t>
+  </si>
+  <si>
+    <t>could be done by re-running clean versions of the metacell scripts.</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -731,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,6 +1130,23 @@
       </c>
       <c r="E26" s="12"/>
     </row>
+    <row r="27" spans="1:5" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1135,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BA4A1-55DF-473D-9C92-55227EF915D8}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Edits Methods and List of Figs/Table for Chapter 3
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51ED9736-CD0D-4251-B091-2F264B2A0891}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635A1624-E60C-40EB-96DE-38D338B1DA56}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
+    <workbookView minimized="1" xWindow="29370" yWindow="570" windowWidth="18000" windowHeight="12615" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentioned_in_text" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>could be done by re-running clean versions of the metacell scripts.</t>
+  </si>
+  <si>
+    <t>Supplementary Table S3.6</t>
+  </si>
+  <si>
+    <t>Ranking process for choosing PRC-like metacells.</t>
   </si>
 </sst>
 </file>
@@ -437,6 +443,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1145,6 +1155,17 @@
       </c>
       <c r="E27" s="14" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing Tables S3.6 and S3.7
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635A1624-E60C-40EB-96DE-38D338B1DA56}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47261959-5CCB-4E2F-B702-7AC8A5943157}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="29370" yWindow="570" windowWidth="18000" windowHeight="12615" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentioned_in_text" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Figure 3.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Cross-species comparison of orthogroups of regulatory genes expressed in PRC-like metacells. </t>
-  </si>
-  <si>
     <t>Figure 3.8</t>
   </si>
   <si>
@@ -274,6 +271,24 @@
   </si>
   <si>
     <t>Ranking process for choosing PRC-like metacells.</t>
+  </si>
+  <si>
+    <t>Supplementary Table S3.7</t>
+  </si>
+  <si>
+    <t>List of known TFs Pfam codes</t>
+  </si>
+  <si>
+    <t>Cross-species comparison of orthogroups of regulatory genes expressed in PRC-like metacells. (heatmap and network)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most common orthogroups of regulatory genes shared across PRC-like metacells throughout animals. </t>
+  </si>
+  <si>
+    <t>More or less prepared. To be added.</t>
+  </si>
+  <si>
+    <t>Found original excel file. It looks in good shape as is.</t>
   </si>
 </sst>
 </file>
@@ -746,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1028,7 +1043,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>14</v>
@@ -1037,13 +1052,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>14</v>
@@ -1052,13 +1067,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>15</v>
@@ -1067,13 +1082,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>15</v>
@@ -1088,10 +1103,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>51</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -1103,22 +1118,22 @@
         <v>16</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>15</v>
@@ -1127,13 +1142,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>15</v>
@@ -1142,31 +1157,52 @@
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="14" t="s">
+    </row>
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="D28" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="C29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1186,22 +1222,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidied up references to supplementary material for reconciliations
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47261959-5CCB-4E2F-B702-7AC8A5943157}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4123E40A-5625-468D-AAF3-42AE7FE2F189}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>Found original excel file. It looks in good shape as is.</t>
+  </si>
+  <si>
+    <t>supplementary files with the full reconciliation for GRK on GitHub</t>
+  </si>
+  <si>
+    <t>supplementary files with the full reconciliation for PLC on GitHub</t>
+  </si>
+  <si>
+    <t>supplementary files with the full reconciliation for opsins on GitHub</t>
   </si>
 </sst>
 </file>
@@ -763,13 +772,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="28.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="110.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.54296875" style="5" customWidth="1"/>
@@ -909,7 +918,7 @@
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>9</v>
@@ -926,7 +935,7 @@
     </row>
     <row r="12" spans="1:5" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>9</v>
@@ -990,7 +999,7 @@
     </row>
     <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Resolving some issues in Chapter 3 manuscript and list of figs/tables
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="218" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4123E40A-5625-468D-AAF3-42AE7FE2F189}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAFA7639-42A2-4EDD-9191-158B4D874DB5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
+    <workbookView minimized="1" xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11265" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentioned_in_text" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -167,9 +167,6 @@
     <t xml:space="preserve">Expression of phototransduction genes in photoreceptor-like cells across animals. </t>
   </si>
   <si>
-    <t>Supplementary Material X</t>
-  </si>
-  <si>
     <t>Refers to material that shows that Dmel met 10 expresses EOMES</t>
   </si>
   <si>
@@ -298,6 +295,12 @@
   </si>
   <si>
     <t>supplementary files with the full reconciliation for opsins on GitHub</t>
+  </si>
+  <si>
+    <t>also at beginning of each metacell scripts I could add a link to where the raw data can be downloaded..</t>
+  </si>
+  <si>
+    <t>list of all genes with their respective lfp values</t>
   </si>
 </sst>
 </file>
@@ -773,7 +776,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -918,7 +921,7 @@
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>9</v>
@@ -935,7 +938,7 @@
     </row>
     <row r="12" spans="1:5" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>9</v>
@@ -982,47 +985,47 @@
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>14</v>
@@ -1031,13 +1034,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>14</v>
@@ -1046,13 +1049,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>14</v>
@@ -1061,13 +1064,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>14</v>
@@ -1076,13 +1079,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>15</v>
@@ -1091,13 +1094,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>15</v>
@@ -1112,10 +1115,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>50</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -1127,22 +1130,22 @@
         <v>16</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>15</v>
@@ -1151,13 +1154,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>15</v>
@@ -1166,47 +1169,47 @@
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>15</v>
@@ -1221,32 +1224,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670BA4A1-55DF-473D-9C92-55227EF915D8}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Chapter 3 Manuscript v2. And made copy (v2.1) for supervisors
</commit_message>
<xml_diff>
--- a/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
+++ b/3_Evolution_of_phototransduction_and_PRCs/List_all_figures_and_tables_chapter_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofleicester-my.sharepoint.com/personal/aa1176_leicester_ac_uk/Documents/THESIS_WRITING_Clone_current/3_Evolution_of_phototransduction_and_PRCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAFA7639-42A2-4EDD-9191-158B4D874DB5}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{05CDE9F0-47B9-4B31-B903-4E198F36DCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88F1DE17-AE9B-48A3-9D82-D16DF9898AC0}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11265" xr2:uid="{012DABF6-378F-4F45-9844-89F798B70B4B}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Figure 3.3</t>
   </si>
   <si>
-    <t>Supplementary Figure X</t>
-  </si>
-  <si>
     <t>NEEDS TO BE PROPERLY PREPAPARED &amp; DECIDED WHERE TO PUT ETC.</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>list of all genes with their respective lfp values</t>
+  </si>
+  <si>
+    <t>are available on GitHub</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8C4C2-2682-4F04-B2E5-A6609D1F7645}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,7 +811,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -912,7 +912,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>14</v>
@@ -921,47 +921,47 @@
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="6" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>14</v>
@@ -970,13 +970,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>14</v>
@@ -985,47 +985,47 @@
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>14</v>
@@ -1034,13 +1034,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>14</v>
@@ -1049,13 +1049,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>14</v>
@@ -1064,13 +1064,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>14</v>
@@ -1079,13 +1079,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>15</v>
@@ -1094,13 +1094,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>15</v>
@@ -1109,43 +1109,43 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>48</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>49</v>
       </c>
       <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>15</v>
@@ -1154,13 +1154,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>15</v>
@@ -1169,47 +1169,47 @@
     </row>
     <row r="27" spans="1:5" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>15</v>
@@ -1234,27 +1234,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>